<commit_message>
add main.py and python requirements file
</commit_message>
<xml_diff>
--- a/src/file_manager/tests/artifacts/20230224_triton_VVB.xlsx
+++ b/src/file_manager/tests/artifacts/20230224_triton_VVB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inlint-my.sharepoint.com/personal/vania_vilasboas_inl_int/Documents/a_Nanosafety/a_lab work/lung models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOA5BRG\Tese Angelina\LabReport\src\file_manager\tests\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{343CEC51-3EEA-B741-8A30-1CC25482ED23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8620500-8CA9-1C4B-861A-D9B1475B0700}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2908BA-BF72-4791-8F82-E2CA399C8AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="18280" windowHeight="12300" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15075" yWindow="-21885" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -554,7 +554,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -942,6 +942,12 @@
     <xf numFmtId="10" fontId="4" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -958,12 +964,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7268,13 +7268,13 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="56" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="63.75">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -7290,13 +7290,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>0.41658564814814819</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>258527</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -7344,13 +7344,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="38.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -7366,13 +7366,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="38.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:99" ht="76.5">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:99" ht="25.5">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -7388,61 +7388,61 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:99">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:99">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:99" ht="42" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:99" ht="51">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:99" ht="25.5">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:99" ht="56" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:99" ht="51">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:99" ht="89.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:99" ht="25.5">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:99">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:99">
       <c r="A28" s="5">
         <v>560590</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="30" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:99" ht="25.5">
       <c r="B30" s="6" t="s">
         <v>8</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:99">
       <c r="B31" s="7">
         <v>0</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:99">
       <c r="B32" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -8330,7 +8330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:99">
       <c r="B33" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:99">
       <c r="B34" s="7">
         <v>3.125E-2</v>
       </c>
@@ -8922,7 +8922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:99">
       <c r="B35" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:99">
       <c r="B36" s="7">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:99">
       <c r="B37" s="7">
         <v>6.25E-2</v>
       </c>
@@ -9810,13 +9810,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:99">
       <c r="A39" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:99">
       <c r="B41" s="9"/>
       <c r="C41" s="6">
         <v>1</v>
@@ -9855,8 +9855,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B42" s="54" t="s">
+    <row r="42" spans="1:99" ht="19.5">
+      <c r="B42" s="56" t="s">
         <v>130</v>
       </c>
       <c r="C42" s="10">
@@ -9899,8 +9899,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B43" s="55"/>
+    <row r="43" spans="1:99" ht="19.5">
+      <c r="B43" s="57"/>
       <c r="C43" s="12">
         <v>1</v>
       </c>
@@ -9941,8 +9941,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B44" s="55"/>
+    <row r="44" spans="1:99" ht="19.5">
+      <c r="B44" s="57"/>
       <c r="C44" s="13">
         <v>5.7291666666666664E-2</v>
       </c>
@@ -9983,8 +9983,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B45" s="56"/>
+    <row r="45" spans="1:99" ht="19.5">
+      <c r="B45" s="58"/>
       <c r="C45" s="14">
         <v>5.1134259259259261E-2</v>
       </c>
@@ -10025,8 +10025,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B46" s="54" t="s">
+    <row r="46" spans="1:99" ht="19.5">
+      <c r="B46" s="56" t="s">
         <v>135</v>
       </c>
       <c r="C46" s="10">
@@ -10069,8 +10069,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B47" s="55"/>
+    <row r="47" spans="1:99" ht="19.5">
+      <c r="B47" s="57"/>
       <c r="C47" s="12">
         <v>1</v>
       </c>
@@ -10111,8 +10111,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B48" s="55"/>
+    <row r="48" spans="1:99" ht="19.5">
+      <c r="B48" s="57"/>
       <c r="C48" s="13">
         <v>5.208333333333333E-3</v>
       </c>
@@ -10153,8 +10153,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B49" s="56"/>
+    <row r="49" spans="2:15" ht="19.5">
+      <c r="B49" s="58"/>
       <c r="C49" s="14">
         <v>0</v>
       </c>
@@ -10195,8 +10195,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B50" s="54" t="s">
+    <row r="50" spans="2:15" ht="19.5">
+      <c r="B50" s="56" t="s">
         <v>136</v>
       </c>
       <c r="C50" s="10">
@@ -10239,8 +10239,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B51" s="55"/>
+    <row r="51" spans="2:15" ht="19.5">
+      <c r="B51" s="57"/>
       <c r="C51" s="12">
         <v>1</v>
       </c>
@@ -10281,8 +10281,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B52" s="55"/>
+    <row r="52" spans="2:15" ht="19.5">
+      <c r="B52" s="57"/>
       <c r="C52" s="13">
         <v>5.208333333333333E-3</v>
       </c>
@@ -10323,8 +10323,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B53" s="56"/>
+    <row r="53" spans="2:15" ht="19.5">
+      <c r="B53" s="58"/>
       <c r="C53" s="14">
         <v>0</v>
       </c>
@@ -10365,8 +10365,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B54" s="54" t="s">
+    <row r="54" spans="2:15" ht="19.5">
+      <c r="B54" s="56" t="s">
         <v>137</v>
       </c>
       <c r="C54" s="10">
@@ -10409,8 +10409,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B55" s="55"/>
+    <row r="55" spans="2:15" ht="19.5">
+      <c r="B55" s="57"/>
       <c r="C55" s="12">
         <v>1</v>
       </c>
@@ -10451,8 +10451,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B56" s="55"/>
+    <row r="56" spans="2:15" ht="19.5">
+      <c r="B56" s="57"/>
       <c r="C56" s="13">
         <v>5.208333333333333E-3</v>
       </c>
@@ -10493,8 +10493,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B57" s="56"/>
+    <row r="57" spans="2:15" ht="19.5">
+      <c r="B57" s="58"/>
       <c r="C57" s="14">
         <v>0</v>
       </c>
@@ -10535,8 +10535,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B58" s="54" t="s">
+    <row r="58" spans="2:15" ht="19.5">
+      <c r="B58" s="56" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="10">
@@ -10579,8 +10579,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B59" s="55"/>
+    <row r="59" spans="2:15" ht="19.5">
+      <c r="B59" s="57"/>
       <c r="C59" s="12">
         <v>1</v>
       </c>
@@ -10621,8 +10621,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B60" s="55"/>
+    <row r="60" spans="2:15" ht="19.5">
+      <c r="B60" s="57"/>
       <c r="C60" s="13">
         <v>5.208333333333333E-3</v>
       </c>
@@ -10663,8 +10663,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B61" s="56"/>
+    <row r="61" spans="2:15" ht="19.5">
+      <c r="B61" s="58"/>
       <c r="C61" s="14">
         <v>0</v>
       </c>
@@ -10705,8 +10705,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B62" s="54" t="s">
+    <row r="62" spans="2:15" ht="19.5">
+      <c r="B62" s="56" t="s">
         <v>139</v>
       </c>
       <c r="C62" s="10">
@@ -10749,8 +10749,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B63" s="55"/>
+    <row r="63" spans="2:15" ht="19.5">
+      <c r="B63" s="57"/>
       <c r="C63" s="12">
         <v>1</v>
       </c>
@@ -10791,8 +10791,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B64" s="55"/>
+    <row r="64" spans="2:15" ht="19.5">
+      <c r="B64" s="57"/>
       <c r="C64" s="13">
         <v>4.6875E-2</v>
       </c>
@@ -10833,8 +10833,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B65" s="56"/>
+    <row r="65" spans="2:15" ht="19.5">
+      <c r="B65" s="58"/>
       <c r="C65" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -10875,8 +10875,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B66" s="54" t="s">
+    <row r="66" spans="2:15" ht="19.5">
+      <c r="B66" s="56" t="s">
         <v>140</v>
       </c>
       <c r="C66" s="10">
@@ -10919,8 +10919,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B67" s="55"/>
+    <row r="67" spans="2:15" ht="19.5">
+      <c r="B67" s="57"/>
       <c r="C67" s="12">
         <v>1</v>
       </c>
@@ -10961,8 +10961,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B68" s="55"/>
+    <row r="68" spans="2:15" ht="19.5">
+      <c r="B68" s="57"/>
       <c r="C68" s="13">
         <v>4.6875E-2</v>
       </c>
@@ -11003,8 +11003,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B69" s="56"/>
+    <row r="69" spans="2:15" ht="19.5">
+      <c r="B69" s="58"/>
       <c r="C69" s="14">
         <v>4.9849537037037039E-2</v>
       </c>
@@ -11045,8 +11045,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B70" s="54" t="s">
+    <row r="70" spans="2:15" ht="19.5">
+      <c r="B70" s="56" t="s">
         <v>141</v>
       </c>
       <c r="C70" s="10">
@@ -11089,8 +11089,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B71" s="55"/>
+    <row r="71" spans="2:15" ht="19.5">
+      <c r="B71" s="57"/>
       <c r="C71" s="12">
         <v>1</v>
       </c>
@@ -11131,8 +11131,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B72" s="55"/>
+    <row r="72" spans="2:15" ht="19.5">
+      <c r="B72" s="57"/>
       <c r="C72" s="13">
         <v>2.6041666666666668E-2</v>
       </c>
@@ -11173,8 +11173,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B73" s="56"/>
+    <row r="73" spans="2:15" ht="19.5">
+      <c r="B73" s="58"/>
       <c r="C73" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -11241,14 +11241,14 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="16"/>
+    <col min="1" max="1" width="20.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -11256,7 +11256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="56" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="63.75">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -11264,13 +11264,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -11278,7 +11278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>0.41658564814814819</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" s="15" t="s">
         <v>11</v>
       </c>
@@ -11310,7 +11310,7 @@
         <v>258527</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -11318,13 +11318,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:2" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="38.25">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
@@ -11340,13 +11340,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" ht="38.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:99" ht="76.5">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
@@ -11354,7 +11354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:99" ht="25.5">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
@@ -11362,61 +11362,61 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:99">
       <c r="A19" s="15"/>
       <c r="B19" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:99">
       <c r="A20" s="15"/>
       <c r="B20" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:99" ht="42" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:99" ht="51">
       <c r="A21" s="15"/>
       <c r="B21" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:99" ht="25.5">
       <c r="A22" s="15"/>
       <c r="B22" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:99" ht="56" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:99" ht="51">
       <c r="A23" s="15"/>
       <c r="B23" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:99" ht="89.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:99" ht="25.5">
       <c r="A25" s="15"/>
       <c r="B25" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:99">
       <c r="A26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="15"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:99">
       <c r="A28" s="20">
         <v>560590</v>
       </c>
       <c r="B28" s="15"/>
     </row>
-    <row r="30" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:99" ht="25.5">
       <c r="B30" s="21" t="s">
         <v>8</v>
       </c>
@@ -11712,7 +11712,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:99">
       <c r="B31" s="22">
         <v>0</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:99">
       <c r="B32" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:99">
       <c r="B33" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -12600,7 +12600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:99">
       <c r="B34" s="22">
         <v>3.125E-2</v>
       </c>
@@ -12896,7 +12896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:99">
       <c r="B35" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -13192,7 +13192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:99">
       <c r="B36" s="22">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -13488,7 +13488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:99">
       <c r="B37" s="22">
         <v>6.25E-2</v>
       </c>
@@ -13784,13 +13784,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:99">
       <c r="A39" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="15"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:99">
       <c r="B41" s="24"/>
       <c r="C41" s="21">
         <v>1</v>
@@ -13829,8 +13829,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B42" s="57" t="s">
+    <row r="42" spans="1:99" ht="19.5">
+      <c r="B42" s="59" t="s">
         <v>130</v>
       </c>
       <c r="C42" s="25">
@@ -13873,8 +13873,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B43" s="58"/>
+    <row r="43" spans="1:99" ht="19.5">
+      <c r="B43" s="60"/>
       <c r="C43" s="27">
         <v>1</v>
       </c>
@@ -13915,8 +13915,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B44" s="58"/>
+    <row r="44" spans="1:99" ht="19.5">
+      <c r="B44" s="60"/>
       <c r="C44" s="28">
         <v>5.7291666666666664E-2</v>
       </c>
@@ -13957,8 +13957,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B45" s="59"/>
+    <row r="45" spans="1:99" ht="19.5">
+      <c r="B45" s="61"/>
       <c r="C45" s="29">
         <v>5.1134259259259261E-2</v>
       </c>
@@ -13999,8 +13999,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B46" s="57" t="s">
+    <row r="46" spans="1:99" ht="19.5">
+      <c r="B46" s="59" t="s">
         <v>135</v>
       </c>
       <c r="C46" s="25">
@@ -14043,8 +14043,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B47" s="58"/>
+    <row r="47" spans="1:99" ht="19.5">
+      <c r="B47" s="60"/>
       <c r="C47" s="27">
         <v>1</v>
       </c>
@@ -14085,8 +14085,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B48" s="58"/>
+    <row r="48" spans="1:99" ht="19.5">
+      <c r="B48" s="60"/>
       <c r="C48" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -14127,8 +14127,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B49" s="59"/>
+    <row r="49" spans="2:15" ht="19.5">
+      <c r="B49" s="61"/>
       <c r="C49" s="29">
         <v>0</v>
       </c>
@@ -14169,8 +14169,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B50" s="57" t="s">
+    <row r="50" spans="2:15" ht="19.5">
+      <c r="B50" s="59" t="s">
         <v>136</v>
       </c>
       <c r="C50" s="25">
@@ -14213,8 +14213,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B51" s="58"/>
+    <row r="51" spans="2:15" ht="19.5">
+      <c r="B51" s="60"/>
       <c r="C51" s="27">
         <v>1</v>
       </c>
@@ -14255,8 +14255,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B52" s="58"/>
+    <row r="52" spans="2:15" ht="19.5">
+      <c r="B52" s="60"/>
       <c r="C52" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -14297,8 +14297,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B53" s="59"/>
+    <row r="53" spans="2:15" ht="19.5">
+      <c r="B53" s="61"/>
       <c r="C53" s="29">
         <v>0</v>
       </c>
@@ -14339,8 +14339,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B54" s="57" t="s">
+    <row r="54" spans="2:15" ht="19.5">
+      <c r="B54" s="59" t="s">
         <v>137</v>
       </c>
       <c r="C54" s="25">
@@ -14383,8 +14383,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B55" s="58"/>
+    <row r="55" spans="2:15" ht="19.5">
+      <c r="B55" s="60"/>
       <c r="C55" s="27">
         <v>1</v>
       </c>
@@ -14425,8 +14425,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B56" s="58"/>
+    <row r="56" spans="2:15" ht="19.5">
+      <c r="B56" s="60"/>
       <c r="C56" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -14467,8 +14467,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B57" s="59"/>
+    <row r="57" spans="2:15" ht="19.5">
+      <c r="B57" s="61"/>
       <c r="C57" s="29">
         <v>0</v>
       </c>
@@ -14509,8 +14509,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B58" s="57" t="s">
+    <row r="58" spans="2:15" ht="19.5">
+      <c r="B58" s="59" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="25">
@@ -14553,8 +14553,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B59" s="58"/>
+    <row r="59" spans="2:15" ht="19.5">
+      <c r="B59" s="60"/>
       <c r="C59" s="27">
         <v>1</v>
       </c>
@@ -14595,8 +14595,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B60" s="58"/>
+    <row r="60" spans="2:15" ht="19.5">
+      <c r="B60" s="60"/>
       <c r="C60" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -14637,8 +14637,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B61" s="59"/>
+    <row r="61" spans="2:15" ht="19.5">
+      <c r="B61" s="61"/>
       <c r="C61" s="29">
         <v>0</v>
       </c>
@@ -14679,8 +14679,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B62" s="57" t="s">
+    <row r="62" spans="2:15" ht="19.5">
+      <c r="B62" s="59" t="s">
         <v>139</v>
       </c>
       <c r="C62" s="25">
@@ -14723,8 +14723,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B63" s="58"/>
+    <row r="63" spans="2:15" ht="19.5">
+      <c r="B63" s="60"/>
       <c r="C63" s="27">
         <v>1</v>
       </c>
@@ -14765,8 +14765,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B64" s="58"/>
+    <row r="64" spans="2:15" ht="19.5">
+      <c r="B64" s="60"/>
       <c r="C64" s="28">
         <v>4.6875E-2</v>
       </c>
@@ -14807,8 +14807,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B65" s="59"/>
+    <row r="65" spans="2:15" ht="19.5">
+      <c r="B65" s="61"/>
       <c r="C65" s="29">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -14849,8 +14849,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B66" s="57" t="s">
+    <row r="66" spans="2:15" ht="19.5">
+      <c r="B66" s="59" t="s">
         <v>140</v>
       </c>
       <c r="C66" s="25">
@@ -14893,8 +14893,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B67" s="58"/>
+    <row r="67" spans="2:15" ht="19.5">
+      <c r="B67" s="60"/>
       <c r="C67" s="27">
         <v>1</v>
       </c>
@@ -14935,8 +14935,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B68" s="58"/>
+    <row r="68" spans="2:15" ht="19.5">
+      <c r="B68" s="60"/>
       <c r="C68" s="28">
         <v>4.6875E-2</v>
       </c>
@@ -14977,8 +14977,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B69" s="59"/>
+    <row r="69" spans="2:15" ht="19.5">
+      <c r="B69" s="61"/>
       <c r="C69" s="29">
         <v>4.9849537037037039E-2</v>
       </c>
@@ -15019,8 +15019,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B70" s="57" t="s">
+    <row r="70" spans="2:15" ht="19.5">
+      <c r="B70" s="59" t="s">
         <v>141</v>
       </c>
       <c r="C70" s="25">
@@ -15063,8 +15063,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B71" s="58"/>
+    <row r="71" spans="2:15" ht="19.5">
+      <c r="B71" s="60"/>
       <c r="C71" s="27">
         <v>1</v>
       </c>
@@ -15105,8 +15105,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B72" s="58"/>
+    <row r="72" spans="2:15" ht="19.5">
+      <c r="B72" s="60"/>
       <c r="C72" s="28">
         <v>2.6041666666666668E-2</v>
       </c>
@@ -15147,8 +15147,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B73" s="59"/>
+    <row r="73" spans="2:15" ht="19.5">
+      <c r="B73" s="61"/>
       <c r="C73" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -15209,23 +15209,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:CU175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="L137" sqref="L137"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="16" customWidth="1"/>
-    <col min="3" max="4" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="9.1640625" style="16"/>
-    <col min="12" max="12" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="16"/>
-    <col min="14" max="14" width="13.5" style="16" customWidth="1"/>
-    <col min="15" max="16384" width="9.1640625" style="16"/>
+    <col min="1" max="1" width="10.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="16" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="9.140625" style="16"/>
+    <col min="12" max="12" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="16"/>
+    <col min="14" max="14" width="13.42578125" style="16" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -15233,7 +15233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="63.75">
       <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
@@ -15244,13 +15244,13 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="25.5">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="25.5">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -15258,7 +15258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
@@ -15266,7 +15266,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -15274,7 +15274,7 @@
         <v>0.41658564814814819</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -15282,7 +15282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="38.25">
       <c r="A10" s="15" t="s">
         <v>11</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>258527</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="25.5">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
@@ -15298,13 +15298,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="25.5">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="38.25">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="38.25">
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
@@ -15320,13 +15320,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="38.25">
       <c r="A16" s="15"/>
       <c r="B16" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:99" ht="76.5">
       <c r="A17" s="15" t="s">
         <v>20</v>
       </c>
@@ -15334,7 +15334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:99" ht="25.5">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
@@ -15342,61 +15342,61 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:99">
       <c r="A19" s="15"/>
       <c r="B19" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:99">
       <c r="A20" s="15"/>
       <c r="B20" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:99" ht="42" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:99" ht="51">
       <c r="A21" s="15"/>
       <c r="B21" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:99" ht="25.5">
       <c r="A22" s="15"/>
       <c r="B22" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:99" ht="56" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:99" ht="51">
       <c r="A23" s="15"/>
       <c r="B23" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:99" ht="84" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:99" ht="89.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:99" ht="28" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:99" ht="25.5">
       <c r="A25" s="15"/>
       <c r="B25" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:99" ht="25.5">
       <c r="A26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="15"/>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:99">
       <c r="A28" s="20">
         <v>560590</v>
       </c>
       <c r="B28" s="15"/>
     </row>
-    <row r="30" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:99">
       <c r="B30" s="21" t="s">
         <v>8</v>
       </c>
@@ -15692,7 +15692,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:99">
       <c r="B31" s="22">
         <v>0</v>
       </c>
@@ -15988,7 +15988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:99">
       <c r="B32" s="22">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -16284,7 +16284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:99">
       <c r="B33" s="22">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -16580,7 +16580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:99">
       <c r="B34" s="22">
         <v>3.125E-2</v>
       </c>
@@ -16876,7 +16876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:99">
       <c r="B35" s="22">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -17172,7 +17172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:99">
       <c r="B36" s="22">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -17468,7 +17468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:99">
       <c r="B37" s="22">
         <v>6.25E-2</v>
       </c>
@@ -17764,13 +17764,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:99" ht="14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:99">
       <c r="A39" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B39" s="15"/>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:99">
       <c r="B41" s="24"/>
       <c r="C41" s="21">
         <v>1</v>
@@ -17809,8 +17809,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B42" s="57" t="s">
+    <row r="42" spans="1:99" ht="19.5">
+      <c r="B42" s="59" t="s">
         <v>130</v>
       </c>
       <c r="C42" s="25">
@@ -17853,8 +17853,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B43" s="58"/>
+    <row r="43" spans="1:99" ht="19.5">
+      <c r="B43" s="60"/>
       <c r="C43" s="27">
         <v>1</v>
       </c>
@@ -17895,8 +17895,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="44" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B44" s="58"/>
+    <row r="44" spans="1:99" ht="19.5">
+      <c r="B44" s="60"/>
       <c r="C44" s="28">
         <v>5.7291666666666664E-2</v>
       </c>
@@ -17937,8 +17937,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B45" s="59"/>
+    <row r="45" spans="1:99" ht="19.5">
+      <c r="B45" s="61"/>
       <c r="C45" s="29">
         <v>5.1134259259259261E-2</v>
       </c>
@@ -17979,8 +17979,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B46" s="57" t="s">
+    <row r="46" spans="1:99" ht="19.5">
+      <c r="B46" s="59" t="s">
         <v>135</v>
       </c>
       <c r="C46" s="25">
@@ -18023,8 +18023,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B47" s="58"/>
+    <row r="47" spans="1:99" ht="19.5">
+      <c r="B47" s="60"/>
       <c r="C47" s="27">
         <v>1</v>
       </c>
@@ -18065,8 +18065,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:99" ht="24" x14ac:dyDescent="0.15">
-      <c r="B48" s="58"/>
+    <row r="48" spans="1:99" ht="19.5">
+      <c r="B48" s="60"/>
       <c r="C48" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -18107,8 +18107,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B49" s="59"/>
+    <row r="49" spans="2:15" ht="19.5">
+      <c r="B49" s="61"/>
       <c r="C49" s="29">
         <v>0</v>
       </c>
@@ -18149,8 +18149,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B50" s="57" t="s">
+    <row r="50" spans="2:15" ht="19.5">
+      <c r="B50" s="59" t="s">
         <v>136</v>
       </c>
       <c r="C50" s="25">
@@ -18193,8 +18193,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B51" s="58"/>
+    <row r="51" spans="2:15" ht="19.5">
+      <c r="B51" s="60"/>
       <c r="C51" s="27">
         <v>1</v>
       </c>
@@ -18235,8 +18235,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B52" s="58"/>
+    <row r="52" spans="2:15" ht="19.5">
+      <c r="B52" s="60"/>
       <c r="C52" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -18277,8 +18277,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B53" s="59"/>
+    <row r="53" spans="2:15" ht="19.5">
+      <c r="B53" s="61"/>
       <c r="C53" s="29">
         <v>0</v>
       </c>
@@ -18319,8 +18319,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B54" s="57" t="s">
+    <row r="54" spans="2:15" ht="19.5">
+      <c r="B54" s="59" t="s">
         <v>137</v>
       </c>
       <c r="C54" s="25">
@@ -18363,8 +18363,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B55" s="58"/>
+    <row r="55" spans="2:15" ht="19.5">
+      <c r="B55" s="60"/>
       <c r="C55" s="27">
         <v>1</v>
       </c>
@@ -18405,8 +18405,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B56" s="58"/>
+    <row r="56" spans="2:15" ht="19.5">
+      <c r="B56" s="60"/>
       <c r="C56" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -18447,8 +18447,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B57" s="59"/>
+    <row r="57" spans="2:15" ht="19.5">
+      <c r="B57" s="61"/>
       <c r="C57" s="29">
         <v>0</v>
       </c>
@@ -18489,8 +18489,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B58" s="57" t="s">
+    <row r="58" spans="2:15" ht="19.5">
+      <c r="B58" s="59" t="s">
         <v>138</v>
       </c>
       <c r="C58" s="25">
@@ -18533,8 +18533,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B59" s="58"/>
+    <row r="59" spans="2:15" ht="19.5">
+      <c r="B59" s="60"/>
       <c r="C59" s="27">
         <v>1</v>
       </c>
@@ -18575,8 +18575,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B60" s="58"/>
+    <row r="60" spans="2:15" ht="19.5">
+      <c r="B60" s="60"/>
       <c r="C60" s="28">
         <v>5.208333333333333E-3</v>
       </c>
@@ -18617,8 +18617,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B61" s="59"/>
+    <row r="61" spans="2:15" ht="19.5">
+      <c r="B61" s="61"/>
       <c r="C61" s="29">
         <v>0</v>
       </c>
@@ -18659,8 +18659,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B62" s="57" t="s">
+    <row r="62" spans="2:15" ht="19.5">
+      <c r="B62" s="59" t="s">
         <v>139</v>
       </c>
       <c r="C62" s="25">
@@ -18703,8 +18703,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B63" s="58"/>
+    <row r="63" spans="2:15" ht="19.5">
+      <c r="B63" s="60"/>
       <c r="C63" s="27">
         <v>1</v>
       </c>
@@ -18745,8 +18745,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="2:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B64" s="58"/>
+    <row r="64" spans="2:15" ht="19.5">
+      <c r="B64" s="60"/>
       <c r="C64" s="28">
         <v>4.6875E-2</v>
       </c>
@@ -18787,8 +18787,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B65" s="59"/>
+    <row r="65" spans="1:15" ht="19.5">
+      <c r="B65" s="61"/>
       <c r="C65" s="29">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -18829,8 +18829,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B66" s="57" t="s">
+    <row r="66" spans="1:15" ht="19.5">
+      <c r="B66" s="59" t="s">
         <v>140</v>
       </c>
       <c r="C66" s="25">
@@ -18873,8 +18873,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B67" s="58"/>
+    <row r="67" spans="1:15" ht="19.5">
+      <c r="B67" s="60"/>
       <c r="C67" s="27">
         <v>1</v>
       </c>
@@ -18915,8 +18915,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B68" s="58"/>
+    <row r="68" spans="1:15" ht="19.5">
+      <c r="B68" s="60"/>
       <c r="C68" s="28">
         <v>4.6875E-2</v>
       </c>
@@ -18957,8 +18957,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B69" s="59"/>
+    <row r="69" spans="1:15" ht="19.5">
+      <c r="B69" s="61"/>
       <c r="C69" s="29">
         <v>4.9849537037037039E-2</v>
       </c>
@@ -18999,8 +18999,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B70" s="57" t="s">
+    <row r="70" spans="1:15" ht="19.5">
+      <c r="B70" s="59" t="s">
         <v>141</v>
       </c>
       <c r="C70" s="25">
@@ -19043,8 +19043,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B71" s="58"/>
+    <row r="71" spans="1:15" ht="19.5">
+      <c r="B71" s="60"/>
       <c r="C71" s="27">
         <v>1</v>
       </c>
@@ -19085,8 +19085,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B72" s="58"/>
+    <row r="72" spans="1:15" ht="19.5">
+      <c r="B72" s="60"/>
       <c r="C72" s="28">
         <v>2.6041666666666668E-2</v>
       </c>
@@ -19127,8 +19127,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="24" x14ac:dyDescent="0.15">
-      <c r="B73" s="59"/>
+    <row r="73" spans="1:15" ht="19.5">
+      <c r="B73" s="61"/>
       <c r="C73" s="29">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -19169,7 +19169,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:15">
       <c r="A75" s="9"/>
       <c r="B75" s="6">
         <v>1</v>
@@ -19209,7 +19209,7 @@
       </c>
       <c r="N75"/>
     </row>
-    <row r="76" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:15">
       <c r="A76" s="6" t="s">
         <v>130</v>
       </c>
@@ -19229,7 +19229,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:15">
       <c r="A77" s="6" t="s">
         <v>135</v>
       </c>
@@ -19249,7 +19249,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:15">
       <c r="A78" s="6" t="s">
         <v>136</v>
       </c>
@@ -19269,7 +19269,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:15">
       <c r="A79" s="6" t="s">
         <v>137</v>
       </c>
@@ -19289,7 +19289,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="14" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:15">
       <c r="A80" s="6" t="s">
         <v>138</v>
       </c>
@@ -19309,7 +19309,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:14">
       <c r="A81" s="6" t="s">
         <v>139</v>
       </c>
@@ -19329,7 +19329,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:14">
       <c r="A82" s="6" t="s">
         <v>140</v>
       </c>
@@ -19349,7 +19349,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:14">
       <c r="A83" s="6" t="s">
         <v>141</v>
       </c>
@@ -19369,7 +19369,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:14">
       <c r="A85" s="50" t="s">
         <v>157</v>
       </c>
@@ -19411,11 +19411,11 @@
       </c>
       <c r="N85"/>
     </row>
-    <row r="86" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:14">
       <c r="A86" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B86" s="60">
+      <c r="B86" s="54">
         <v>778</v>
       </c>
       <c r="C86" s="32">
@@ -19445,7 +19445,7 @@
       <c r="K86" s="32">
         <v>2917</v>
       </c>
-      <c r="L86" s="61">
+      <c r="L86" s="55">
         <v>3608</v>
       </c>
       <c r="M86" s="31">
@@ -19455,7 +19455,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:14">
       <c r="A87" s="6" t="s">
         <v>136</v>
       </c>
@@ -19489,7 +19489,7 @@
       <c r="K87" s="32">
         <v>2971</v>
       </c>
-      <c r="L87" s="61">
+      <c r="L87" s="55">
         <v>4111</v>
       </c>
       <c r="M87" s="31">
@@ -19499,7 +19499,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:14">
       <c r="A88" s="6" t="s">
         <v>137</v>
       </c>
@@ -19543,7 +19543,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:14">
       <c r="A89" s="6" t="s">
         <v>138</v>
       </c>
@@ -19588,7 +19588,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:14">
       <c r="A90" s="6" t="s">
         <v>139</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:14">
       <c r="A91" s="6" t="s">
         <v>140</v>
       </c>
@@ -19678,7 +19678,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:14">
       <c r="A92" s="6" t="s">
         <v>151</v>
       </c>
@@ -19688,7 +19688,7 @@
         <v>2956</v>
       </c>
       <c r="D92" s="46">
-        <f t="shared" ref="D92:L92" si="0">AVERAGE(D86:D91)</f>
+        <f t="shared" ref="D92:K92" si="0">AVERAGE(D86:D91)</f>
         <v>3031.3333333333335</v>
       </c>
       <c r="E92" s="46">
@@ -19726,7 +19726,7 @@
       <c r="M92" s="31"/>
       <c r="N92" s="11"/>
     </row>
-    <row r="93" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:14">
       <c r="A93" s="6" t="s">
         <v>152</v>
       </c>
@@ -19736,7 +19736,7 @@
         <v>231.87237869138275</v>
       </c>
       <c r="D93" s="31">
-        <f t="shared" ref="D93:L93" si="1">STDEV(D86:D91)</f>
+        <f t="shared" ref="D93:K93" si="1">STDEV(D86:D91)</f>
         <v>288.23786473443539</v>
       </c>
       <c r="E93" s="31">
@@ -19774,7 +19774,7 @@
       <c r="M93" s="31"/>
       <c r="N93" s="11"/>
     </row>
-    <row r="94" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:14">
       <c r="A94" s="6" t="s">
         <v>153</v>
       </c>
@@ -19822,7 +19822,7 @@
       <c r="M94" s="31"/>
       <c r="N94" s="11"/>
     </row>
-    <row r="95" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:14">
       <c r="A95" s="47" t="s">
         <v>154</v>
       </c>
@@ -19870,7 +19870,7 @@
       <c r="M95" s="48"/>
       <c r="N95" s="11"/>
     </row>
-    <row r="96" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:14">
       <c r="A96" s="47" t="s">
         <v>155</v>
       </c>
@@ -19918,7 +19918,7 @@
       <c r="M96" s="48"/>
       <c r="N96" s="11"/>
     </row>
-    <row r="98" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:14">
       <c r="A98" s="50" t="s">
         <v>158</v>
       </c>
@@ -19960,7 +19960,7 @@
       </c>
       <c r="N98"/>
     </row>
-    <row r="99" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:14">
       <c r="A99" s="6" t="s">
         <v>135</v>
       </c>
@@ -20004,7 +20004,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:14">
       <c r="A100" s="6" t="s">
         <v>136</v>
       </c>
@@ -20048,7 +20048,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:14">
       <c r="A101" s="6" t="s">
         <v>137</v>
       </c>
@@ -20092,7 +20092,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:14">
       <c r="A102" s="6" t="s">
         <v>138</v>
       </c>
@@ -20137,7 +20137,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:14">
       <c r="A103" s="6" t="s">
         <v>139</v>
       </c>
@@ -20182,7 +20182,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:14">
       <c r="A104" s="6" t="s">
         <v>140</v>
       </c>
@@ -20227,7 +20227,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:14">
       <c r="A105" s="6" t="s">
         <v>151</v>
       </c>
@@ -20274,7 +20274,7 @@
       </c>
       <c r="M105" s="31"/>
     </row>
-    <row r="106" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:14">
       <c r="A106" s="6" t="s">
         <v>152</v>
       </c>
@@ -20322,7 +20322,7 @@
       <c r="M106" s="31"/>
       <c r="N106"/>
     </row>
-    <row r="107" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:14">
       <c r="A107" s="6" t="s">
         <v>153</v>
       </c>
@@ -20372,7 +20372,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:14">
       <c r="A108" s="47" t="s">
         <v>154</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:14">
       <c r="A109" s="47" t="s">
         <v>155</v>
       </c>
@@ -20472,12 +20472,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:14">
       <c r="N110" s="11" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:14">
       <c r="A111" s="50" t="s">
         <v>164</v>
       </c>
@@ -20521,7 +20521,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
         <v>135</v>
       </c>
@@ -20565,7 +20565,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:14">
       <c r="A113" s="6" t="s">
         <v>136</v>
       </c>
@@ -20606,7 +20606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:14">
       <c r="A114" s="6" t="s">
         <v>137</v>
       </c>
@@ -20648,7 +20648,7 @@
       </c>
       <c r="N114"/>
     </row>
-    <row r="115" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:14">
       <c r="A115" s="6" t="s">
         <v>138</v>
       </c>
@@ -20693,7 +20693,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:14">
       <c r="A116" s="6" t="s">
         <v>139</v>
       </c>
@@ -20738,7 +20738,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:14">
       <c r="A117" s="6" t="s">
         <v>140</v>
       </c>
@@ -20783,7 +20783,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:14">
       <c r="A118" s="6" t="s">
         <v>151</v>
       </c>
@@ -20830,7 +20830,7 @@
       </c>
       <c r="M118" s="31"/>
     </row>
-    <row r="119" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:14">
       <c r="A119" s="6" t="s">
         <v>152</v>
       </c>
@@ -20878,7 +20878,7 @@
       <c r="M119" s="31"/>
       <c r="N119"/>
     </row>
-    <row r="120" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:14">
       <c r="A120" s="6" t="s">
         <v>153</v>
       </c>
@@ -20928,7 +20928,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:14">
       <c r="A121" s="47" t="s">
         <v>154</v>
       </c>
@@ -20978,7 +20978,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:14">
       <c r="A122" s="47" t="s">
         <v>155</v>
       </c>
@@ -21028,12 +21028,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:14">
       <c r="N123" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:14">
       <c r="A124" s="50" t="s">
         <v>165</v>
       </c>
@@ -21077,7 +21077,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:14">
       <c r="A125" s="6" t="s">
         <v>135</v>
       </c>
@@ -21121,7 +21121,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:14">
       <c r="A126" s="6" t="s">
         <v>136</v>
       </c>
@@ -21162,7 +21162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:14">
       <c r="A127" s="6" t="s">
         <v>137</v>
       </c>
@@ -21204,7 +21204,7 @@
       </c>
       <c r="N127"/>
     </row>
-    <row r="128" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:14">
       <c r="A128" s="6" t="s">
         <v>138</v>
       </c>
@@ -21249,7 +21249,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:14">
       <c r="A129" s="6" t="s">
         <v>139</v>
       </c>
@@ -21294,7 +21294,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:14">
       <c r="A130" s="6" t="s">
         <v>140</v>
       </c>
@@ -21339,7 +21339,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:14">
       <c r="A131" s="6" t="s">
         <v>151</v>
       </c>
@@ -21386,7 +21386,7 @@
       </c>
       <c r="M131" s="31"/>
     </row>
-    <row r="132" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:14">
       <c r="A132" s="6" t="s">
         <v>152</v>
       </c>
@@ -21434,7 +21434,7 @@
       <c r="M132" s="31"/>
       <c r="N132"/>
     </row>
-    <row r="133" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:14">
       <c r="A133" s="6" t="s">
         <v>153</v>
       </c>
@@ -21484,7 +21484,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:14">
       <c r="A134" s="47" t="s">
         <v>154</v>
       </c>
@@ -21534,7 +21534,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:14">
       <c r="A135" s="47" t="s">
         <v>155</v>
       </c>
@@ -21584,7 +21584,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:14">
       <c r="L136" s="16" t="s">
         <v>169</v>
       </c>
@@ -21592,7 +21592,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:14" ht="24" customHeight="1">
       <c r="A137" s="51" t="s">
         <v>166</v>
       </c>
@@ -21636,7 +21636,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:14">
       <c r="A138" s="6" t="s">
         <v>135</v>
       </c>
@@ -21680,7 +21680,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:14">
       <c r="A139" s="6" t="s">
         <v>136</v>
       </c>
@@ -21721,7 +21721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:14">
       <c r="A140" s="6" t="s">
         <v>137</v>
       </c>
@@ -21763,7 +21763,7 @@
       </c>
       <c r="N140"/>
     </row>
-    <row r="141" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:14">
       <c r="A141" s="6" t="s">
         <v>138</v>
       </c>
@@ -21808,7 +21808,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:14">
       <c r="A142" s="6" t="s">
         <v>139</v>
       </c>
@@ -21853,7 +21853,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:14">
       <c r="A143" s="6" t="s">
         <v>140</v>
       </c>
@@ -21898,7 +21898,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:14">
       <c r="A144" s="6" t="s">
         <v>151</v>
       </c>
@@ -21945,7 +21945,7 @@
       </c>
       <c r="M144" s="31"/>
     </row>
-    <row r="145" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:14">
       <c r="A145" s="6" t="s">
         <v>152</v>
       </c>
@@ -21993,7 +21993,7 @@
       <c r="M145" s="31"/>
       <c r="N145"/>
     </row>
-    <row r="146" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:14">
       <c r="A146" s="6" t="s">
         <v>153</v>
       </c>
@@ -22043,7 +22043,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:14">
       <c r="A147" s="47" t="s">
         <v>154</v>
       </c>
@@ -22093,7 +22093,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:14">
       <c r="A148" s="47" t="s">
         <v>155</v>
       </c>
@@ -22143,12 +22143,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:14">
       <c r="N149" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:14" ht="24" customHeight="1">
       <c r="A150" s="51" t="s">
         <v>167</v>
       </c>
@@ -22192,7 +22192,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:14">
       <c r="A151" s="6" t="s">
         <v>135</v>
       </c>
@@ -22236,7 +22236,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:14">
       <c r="A152" s="6" t="s">
         <v>136</v>
       </c>
@@ -22277,7 +22277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:14">
       <c r="A153" s="6" t="s">
         <v>137</v>
       </c>
@@ -22319,7 +22319,7 @@
       </c>
       <c r="N153"/>
     </row>
-    <row r="154" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:14">
       <c r="A154" s="6" t="s">
         <v>138</v>
       </c>
@@ -22364,7 +22364,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:14">
       <c r="A155" s="6" t="s">
         <v>139</v>
       </c>
@@ -22409,7 +22409,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:14">
       <c r="A156" s="6" t="s">
         <v>140</v>
       </c>
@@ -22454,7 +22454,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:14">
       <c r="A157" s="6" t="s">
         <v>151</v>
       </c>
@@ -22501,7 +22501,7 @@
       </c>
       <c r="M157" s="31"/>
     </row>
-    <row r="158" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:14">
       <c r="A158" s="6" t="s">
         <v>152</v>
       </c>
@@ -22549,7 +22549,7 @@
       <c r="M158" s="31"/>
       <c r="N158"/>
     </row>
-    <row r="159" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:14">
       <c r="A159" s="6" t="s">
         <v>153</v>
       </c>
@@ -22599,7 +22599,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:14">
       <c r="A160" s="47" t="s">
         <v>154</v>
       </c>
@@ -22649,7 +22649,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:14">
       <c r="A161" s="47" t="s">
         <v>155</v>
       </c>
@@ -22699,12 +22699,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:14">
       <c r="N162" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:14" ht="24" customHeight="1">
       <c r="A163" s="51" t="s">
         <v>168</v>
       </c>
@@ -22748,7 +22748,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:14">
       <c r="A164" s="6" t="s">
         <v>135</v>
       </c>
@@ -22792,7 +22792,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:14">
       <c r="A165" s="6" t="s">
         <v>136</v>
       </c>
@@ -22833,7 +22833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:14">
       <c r="A166" s="6" t="s">
         <v>137</v>
       </c>
@@ -22875,7 +22875,7 @@
       </c>
       <c r="N166"/>
     </row>
-    <row r="167" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:14">
       <c r="A167" s="6" t="s">
         <v>138</v>
       </c>
@@ -22920,7 +22920,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:14">
       <c r="A168" s="6" t="s">
         <v>139</v>
       </c>
@@ -22965,7 +22965,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:14">
       <c r="A169" s="6" t="s">
         <v>140</v>
       </c>
@@ -23010,7 +23010,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:14">
       <c r="A170" s="6" t="s">
         <v>151</v>
       </c>
@@ -23057,7 +23057,7 @@
       </c>
       <c r="M170" s="31"/>
     </row>
-    <row r="171" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:14">
       <c r="A171" s="6" t="s">
         <v>152</v>
       </c>
@@ -23105,7 +23105,7 @@
       <c r="M171" s="31"/>
       <c r="N171"/>
     </row>
-    <row r="172" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:14">
       <c r="A172" s="6" t="s">
         <v>153</v>
       </c>
@@ -23155,7 +23155,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:14">
       <c r="A173" s="47" t="s">
         <v>154</v>
       </c>
@@ -23205,7 +23205,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:14">
       <c r="A174" s="47" t="s">
         <v>155</v>
       </c>
@@ -23255,7 +23255,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:14">
       <c r="N175" s="11"/>
     </row>
   </sheetData>
@@ -23270,7 +23270,8 @@
     <mergeCell ref="B62:B65"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>